<commit_message>
1. Atualização do Requirements Gateway devido a bloqueio de edição do arquivo
</commit_message>
<xml_diff>
--- a/documentation/Documentação do Diagrama de Caso de Uso.xlsx
+++ b/documentation/Documentação do Diagrama de Caso de Uso.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19105"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B523141-5D39-4401-8D5D-7DB07258820B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Multiplayer Match" sheetId="3" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="87">
   <si>
     <t>Nome do Caso de Uso</t>
   </si>
@@ -280,13 +279,25 @@
   </si>
   <si>
     <t>2. Indicar lista de regras e instruções</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Reference Attribute</t>
+  </si>
+  <si>
+    <t>[Covers: REQ02]</t>
+  </si>
+  <si>
+    <t>(*High)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +317,16 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -366,21 +387,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -412,7 +437,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="">
+        <xdr:cNvPr id="2" name="Imagem 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1756E17-ABC0-4E1D-8FDB-C053F3B717D2}"/>
@@ -707,19 +732,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CEAC00-351F-4E21-9668-2E7A964C5ECD}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{BADD9257-69C2-5333-AA3E-DACA0CB56E37}">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
     <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -727,13 +752,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -741,15 +766,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="Q4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -759,8 +790,14 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
+      <c r="Q5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -771,19 +808,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -791,7 +828,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>16</v>
@@ -800,7 +837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>17</v>
@@ -809,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -818,7 +855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>19</v>
@@ -827,8 +864,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -838,8 +875,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75">
-      <c r="A15" s="3"/>
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
@@ -857,19 +894,19 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DB3BC7-9D24-4893-9D6B-30439A40D5D3}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{D14229EF-D285-5147-9107-42FA8977C4BC}">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -877,27 +914,39 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
+      <c r="I3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="I4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -908,7 +957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -916,13 +965,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -930,7 +979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>77</v>
       </c>
@@ -938,7 +987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>78</v>
@@ -947,14 +996,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
       <c r="B12" s="1"/>
     </row>
   </sheetData>
@@ -967,19 +1016,19 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3539A56-6EC7-4557-9A01-A3BE147B490C}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{DE4610C6-C918-5CA0-8E0B-34C58624DADC}">
-      <selection sqref="A1:B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -987,27 +1036,39 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
+      <c r="I3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="I4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1018,19 +1079,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1038,7 +1099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>81</v>
       </c>
@@ -1046,7 +1107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>82</v>
@@ -1055,14 +1116,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
       <c r="B12" s="1"/>
     </row>
   </sheetData>
@@ -1075,14 +1136,34 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234E0856-34FE-411E-9411-BF1E2DC8BD7E}">
-  <dimension ref="A1"/>
+  <dimension ref="S7:T8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{2F3339F5-B212-50F6-BBA6-925B5C44AC27}">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S7" sqref="S7:T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1090,19 +1171,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908F9704-CEE6-4E94-8DBE-98A257530040}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{C7215097-96FC-54F6-922C-B032F8B18F57}">
-      <selection activeCell="A10" sqref="A10:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="94.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1118,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1126,7 +1207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1134,7 +1215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1144,8 +1225,14 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
+      <c r="G5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1155,14 +1242,20 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
+      <c r="G6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1170,7 +1263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1178,8 +1271,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1189,8 +1282,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
-      <c r="A11" s="3"/>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
       <c r="B11" s="1"/>
     </row>
   </sheetData>
@@ -1203,19 +1296,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5ADE9F-AAE9-41A4-A80F-26A95F7B683B}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{B99879BA-EDFB-540C-91CA-3D23971FE62A}">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="96.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="99.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1223,7 +1316,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1231,7 +1324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1239,15 +1332,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="F4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1257,8 +1356,14 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
+      <c r="F5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1269,13 +1374,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1283,34 +1388,34 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1324,19 +1429,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E89FAE-08B9-4B5E-B7A1-0DA6B2B14D7F}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{7F82679C-9042-57F1-8F8E-1FD0C02E8DBA}">
-      <selection sqref="A1:B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="73.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1344,13 +1449,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1358,15 +1463,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="L4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1376,8 +1487,14 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
+      <c r="L5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1388,13 +1505,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1402,7 +1519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>16</v>
@@ -1411,7 +1528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>17</v>
@@ -1420,7 +1537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1429,7 +1546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>19</v>
@@ -1438,8 +1555,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1449,8 +1566,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75">
-      <c r="A14" s="3"/>
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1468,19 +1585,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CA9B47-38BD-4CC3-968E-BBB6A4514843}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{8CC71D4B-B4EE-5E72-98A9-1CF6F3D30EE5}">
-      <selection activeCell="B13" sqref="A1:B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="101.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1488,13 +1605,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1502,13 +1619,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1518,16 +1635,28 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
+      <c r="H5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
+      <c r="H6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1535,7 +1664,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1543,13 +1672,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -1557,22 +1686,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1587,19 +1716,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99446B4B-113B-4D9D-8385-38CDC97D804C}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{15E5DDCD-F1F4-5C80-9908-18E33FEB4A8E}">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="107.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1607,13 +1736,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1621,13 +1750,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="H4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1637,8 +1772,14 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
+      <c r="H5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1646,13 +1787,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1660,19 +1801,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>54</v>
@@ -1681,16 +1822,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1705,19 +1846,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043215A5-9DCA-49D3-935D-A0FA99C25A7C}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{74016F2B-5673-5A1D-B93A-41C4C80F4F37}">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1725,27 +1866,39 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
+      <c r="I3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="I4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1756,7 +1909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1764,7 +1917,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1772,7 +1925,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1780,26 +1933,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1809,8 +1962,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>63</v>
       </c>
@@ -1828,19 +1981,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE459EF0-0EC8-47A6-944B-67A9362877C2}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{98E81C7D-ECF9-542D-85EA-65B0537B96DE}">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1848,27 +2001,39 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
+      <c r="H3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="H4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1879,7 +2044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1887,13 +2052,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1901,7 +2066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
@@ -1909,7 +2074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>68</v>
@@ -1918,14 +2083,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
       <c r="B12" s="1"/>
     </row>
   </sheetData>
@@ -1938,19 +2103,19 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80C22FE-BA15-42DB-B9D1-4857B4B4FC53}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{0D90881D-F28F-527A-BEDB-20B7A7AF6EAC}">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1958,27 +2123,39 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
+      <c r="I3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="I4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1989,7 +2166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1997,13 +2174,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2011,7 +2188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>72</v>
       </c>
@@ -2019,20 +2196,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
       <c r="B12" s="1"/>
     </row>
   </sheetData>
@@ -2044,6 +2221,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100414245D72892E542A3AB118CC6FEC8C3" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cb074634b2e7aa7223c673874ca90f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="21a35b93-b557-48df-8efb-4a4d71b67cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea3fcd82d8fc0eba519ce58ee9b2fe11" ns2:_="">
     <xsd:import namespace="21a35b93-b557-48df-8efb-4a4d71b67cd6"/>
@@ -2193,29 +2385,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7468EF1D-3CD6-42D3-91C6-EC3A42AE3CD9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B79135E-9BCE-4E18-B26C-7F91274352F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="21a35b93-b557-48df-8efb-4a4d71b67cd6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{349303D4-B9B0-424D-99B4-A5C35F2F70B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{349303D4-B9B0-424D-99B4-A5C35F2F70B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B79135E-9BCE-4E18-B26C-7F91274352F7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7468EF1D-3CD6-42D3-91C6-EC3A42AE3CD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="21a35b93-b557-48df-8efb-4a4d71b67cd6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1. Adição do MVP Planning no projeto; 2. Atualização de requisitos cobertos pelo Requirements Gateway - RG não estão reconhecendo alterações no arquivo automaticamente. Mesmo que entenda que LabVIEW e Excel estão cumprindo requisitos, ele não atualiza no Overall Quality
</commit_message>
<xml_diff>
--- a/documentation/Documentação do Diagrama de Caso de Uso.xlsx
+++ b/documentation/Documentação do Diagrama de Caso de Uso.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CE6A2F-B728-4CC7-9FB6-83BEB7D65836}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="88">
   <si>
     <t>Nome do Caso de Uso</t>
   </si>
@@ -291,6 +292,9 @@
   </si>
   <si>
     <t>(*High)</t>
+  </si>
+  <si>
+    <t>[Covers: REQ01]</t>
   </si>
 </sst>
 </file>
@@ -735,13 +739,14 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="Q7" sqref="Q7:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
     <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -813,12 +818,24 @@
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="Q7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1"/>
+      <c r="Q8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2221,18 +2238,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2386,6 +2403,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{349303D4-B9B0-424D-99B4-A5C35F2F70B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B79135E-9BCE-4E18-B26C-7F91274352F7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2397,14 +2422,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{349303D4-B9B0-424D-99B4-A5C35F2F70B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>